<commit_message>
Ajustando responsividade das páginas.
</commit_message>
<xml_diff>
--- a/doc/burndown/burndown.xlsx
+++ b/doc/burndown/burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mclaralvs\Documents\api;\Repositório\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mclaralvs\Documents\api;\Repositório\doc\burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D20B278-59AE-4C06-9697-CA1E894E44B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F354757-B9DB-4E12-9D4F-19E996272ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="16650" yWindow="2145" windowWidth="9135" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Matheus/Fernado</t>
   </si>
   <si>
-    <t>Lay-out das interfaces</t>
-  </si>
-  <si>
     <t>Mariana/Gizeli</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>Data término</t>
+  </si>
+  <si>
+    <t>Layout das interfaces</t>
   </si>
 </sst>
 </file>
@@ -263,16 +263,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,9 +851,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6305550" cy="3533775"/>
     <xdr:graphicFrame macro="">
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:N1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="A30" sqref="A30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="E1" s="2">
         <f ca="1">TODAY()</f>
-        <v>44458</v>
+        <v>44460</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -1490,7 +1490,7 @@
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="19"/>
@@ -1505,7 +1505,7 @@
       <c r="K27" s="20"/>
     </row>
     <row r="28" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="19"/>
@@ -1524,13 +1524,13 @@
         <v>12</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>20</v>
+      <c r="A29" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -1542,7 +1542,7 @@
         <v>44443</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J29" s="12">
         <v>5</v>
@@ -1554,8 +1554,8 @@
       <c r="N29" s="11"/>
     </row>
     <row r="30" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
-        <v>18</v>
+      <c r="A30" s="18" t="s">
+        <v>26</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -1567,7 +1567,7 @@
         <v>44446</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J30" s="12">
         <v>4</v>
@@ -1579,15 +1579,15 @@
       <c r="N30" s="11"/>
     </row>
     <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
       <c r="H31" s="9">
         <v>44452</v>
       </c>
@@ -1603,8 +1603,8 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:14" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
-        <v>22</v>
+      <c r="A32" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -1616,7 +1616,7 @@
         <v>44452</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J32" s="8">
         <v>15</v>
@@ -1626,7 +1626,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="19"/>
@@ -1649,7 +1649,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" s="17" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="19"/>
@@ -1662,7 +1662,7 @@
         <v>44454</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J34" s="12">
         <v>3</v>
@@ -1672,8 +1672,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="25" t="s">
-        <v>24</v>
+      <c r="A35" s="21" t="s">
+        <v>23</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
@@ -1696,7 +1696,7 @@
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="25"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -1710,7 +1710,7 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="22"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -1724,7 +1724,7 @@
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="22"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -1738,7 +1738,7 @@
       <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="22"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -1752,7 +1752,7 @@
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="22"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
@@ -1766,7 +1766,7 @@
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="22"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -1780,7 +1780,7 @@
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="22"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
@@ -1794,7 +1794,7 @@
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="22"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -1808,7 +1808,7 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="22"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
@@ -1822,7 +1822,7 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="22"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -1836,7 +1836,7 @@
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="22"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -1850,7 +1850,7 @@
       <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="22"/>
+      <c r="A47" s="18"/>
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -1864,7 +1864,7 @@
       <c r="L47" s="4"/>
     </row>
     <row r="48" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="22"/>
+      <c r="A48" s="18"/>
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
       <c r="D48" s="19"/>
@@ -1878,7 +1878,7 @@
       <c r="L48" s="4"/>
     </row>
     <row r="49" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="22"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -1892,7 +1892,7 @@
       <c r="L49" s="4"/>
     </row>
     <row r="50" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="22"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
@@ -1906,7 +1906,7 @@
       <c r="L50" s="4"/>
     </row>
     <row r="51" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="22"/>
+      <c r="A51" s="18"/>
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -1920,7 +1920,7 @@
       <c r="L51" s="4"/>
     </row>
     <row r="52" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="22"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
@@ -1934,7 +1934,7 @@
       <c r="L52" s="4"/>
     </row>
     <row r="53" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="22"/>
+      <c r="A53" s="18"/>
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
       <c r="D53" s="19"/>
@@ -1948,7 +1948,7 @@
       <c r="L53" s="4"/>
     </row>
     <row r="54" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="22"/>
+      <c r="A54" s="18"/>
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
       <c r="D54" s="19"/>
@@ -1962,7 +1962,7 @@
       <c r="L54" s="4"/>
     </row>
     <row r="55" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="22"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -1976,7 +1976,7 @@
       <c r="L55" s="4"/>
     </row>
     <row r="56" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="22"/>
+      <c r="A56" s="18"/>
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
@@ -1990,7 +1990,7 @@
       <c r="L56" s="4"/>
     </row>
     <row r="57" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="22"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
       <c r="D57" s="19"/>
@@ -2004,7 +2004,7 @@
       <c r="L57" s="4"/>
     </row>
     <row r="58" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="22"/>
+      <c r="A58" s="18"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
       <c r="D58" s="19"/>
@@ -2018,7 +2018,7 @@
       <c r="L58" s="4"/>
     </row>
     <row r="59" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="22"/>
+      <c r="A59" s="18"/>
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -2032,7 +2032,7 @@
       <c r="L59" s="4"/>
     </row>
     <row r="60" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="22"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
@@ -2046,7 +2046,7 @@
       <c r="L60" s="4"/>
     </row>
     <row r="61" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="22"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -2060,7 +2060,7 @@
       <c r="L61" s="4"/>
     </row>
     <row r="62" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="22"/>
+      <c r="A62" s="18"/>
       <c r="B62" s="19"/>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -2074,7 +2074,7 @@
       <c r="L62" s="4"/>
     </row>
     <row r="63" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="22"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
       <c r="D63" s="19"/>
@@ -2088,7 +2088,7 @@
       <c r="L63" s="4"/>
     </row>
     <row r="64" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="22"/>
+      <c r="A64" s="18"/>
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -2102,7 +2102,7 @@
       <c r="L64" s="4"/>
     </row>
     <row r="65" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="22"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -2116,7 +2116,7 @@
       <c r="L65" s="4"/>
     </row>
     <row r="66" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="22"/>
+      <c r="A66" s="18"/>
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
@@ -2130,7 +2130,7 @@
       <c r="L66" s="4"/>
     </row>
     <row r="67" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="22"/>
+      <c r="A67" s="18"/>
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>
       <c r="D67" s="19"/>
@@ -15305,6 +15305,36 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A63:G63"/>
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="A65:G65"/>
     <mergeCell ref="A66:G66"/>
@@ -15316,36 +15346,6 @@
     <mergeCell ref="A59:G59"/>
     <mergeCell ref="A60:G60"/>
     <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A31:G31"/>
   </mergeCells>
   <conditionalFormatting sqref="I35:J1007">
     <cfRule type="cellIs" dxfId="6" priority="18" operator="greaterThan">
@@ -15388,6 +15388,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F5DCF5D2A3E9D4EB03DE200213EE709" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a88e3926ddc6c6c14365aa5862e4205e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cba8974-30dd-4a7d-8357-6a8b34c8959d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c82f3f457665f9087468efa3d0dd5bf6" ns2:_="">
     <xsd:import namespace="3cba8974-30dd-4a7d-8357-6a8b34c8959d"/>
@@ -15545,15 +15554,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -15561,6 +15561,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6035990A-13B1-4D58-8D05-94F8F1903D6E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B89894DD-E4A8-47EB-941A-377BBE1F4E70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15574,14 +15582,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6035990A-13B1-4D58-8D05-94F8F1903D6E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>